<commit_message>
Adding test plan and sumary to docs folder and other changes
</commit_message>
<xml_diff>
--- a/ui/manual_testing/TestCases_UI.xlsx
+++ b/ui/manual_testing/TestCases_UI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationExercise-QA-Portfolio\1_UI\1_Manual_Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationExercise-QA-Portfolio\ui\manual_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1307,13 +1307,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.77734375" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5546875" style="7" customWidth="1"/>
     <col min="4" max="4" width="33.6640625" style="7" customWidth="1"/>

</xml_diff>

<commit_message>
Add Cypress Automation tests
</commit_message>
<xml_diff>
--- a/ui/manual_testing/TestCases_UI.xlsx
+++ b/ui/manual_testing/TestCases_UI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9528" tabRatio="932"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9528" tabRatio="932" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Signup and Login" sheetId="1" r:id="rId1"/>
@@ -1307,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A3" zoomScale="49" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2039,7 +2039,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2322,7 +2322,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2572,8 +2572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2791,8 +2791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView zoomScale="96" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="96" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>